<commit_message>
Added enterprise logo to Excel and year of the calendar
</commit_message>
<xml_diff>
--- a/2021.xlsx
+++ b/2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\PLB-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\Control-Horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0DF0DE-1DE1-4931-BE05-B085AFC7567B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B40504-AA7B-489E-AF30-F25CA0046B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,14 +400,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -563,7 +555,7 @@
     <t>27 de julio Fiesta en Mataró</t>
   </si>
   <si>
-    <t>MATARÓ</t>
+    <t>Mataró</t>
   </si>
 </sst>
 </file>
@@ -1575,26 +1567,26 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2690,8 +2682,8 @@
   </sheetPr>
   <dimension ref="B1:AC40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2708,15 +2700,15 @@
       <c r="B1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
       <c r="X1" s="53" t="s">
         <v>20</v>
       </c>
@@ -2729,29 +2721,29 @@
     <row r="3" spans="2:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="88" t="s">
+      <c r="L3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="R3" s="4"/>
       <c r="S3" s="5"/>
-      <c r="T3" s="88" t="s">
+      <c r="T3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="90"/>
       <c r="W3" s="5"/>
       <c r="X3" s="6"/>
       <c r="Z3" s="68"/>
@@ -3198,29 +3190,29 @@
     <row r="13" spans="2:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="88" t="s">
+      <c r="L13" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
       <c r="O13" s="5"/>
       <c r="P13" s="6"/>
       <c r="R13" s="4"/>
       <c r="S13" s="5"/>
-      <c r="T13" s="88" t="s">
+      <c r="T13" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="U13" s="89"/>
-      <c r="V13" s="89"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="90"/>
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
     </row>
@@ -3658,29 +3650,29 @@
     <row r="23" spans="2:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
       <c r="J23" s="4"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="88" t="s">
+      <c r="L23" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="89"/>
-      <c r="N23" s="89"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
       <c r="O23" s="5"/>
       <c r="P23" s="6"/>
       <c r="R23" s="4"/>
       <c r="S23" s="5"/>
-      <c r="T23" s="88" t="s">
+      <c r="T23" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="89"/>
-      <c r="V23" s="89"/>
+      <c r="U23" s="90"/>
+      <c r="V23" s="90"/>
       <c r="W23" s="5"/>
       <c r="X23" s="6"/>
       <c r="AA23" s="85" t="s">
@@ -4099,29 +4091,29 @@
     <row r="32" spans="2:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="88" t="s">
+      <c r="D32" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
       <c r="G32" s="5"/>
       <c r="H32" s="6"/>
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="88" t="s">
+      <c r="L32" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="M32" s="89"/>
-      <c r="N32" s="89"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
       <c r="O32" s="5"/>
       <c r="P32" s="6"/>
       <c r="R32" s="4"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="88" t="s">
+      <c r="T32" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="U32" s="89"/>
-      <c r="V32" s="89"/>
+      <c r="U32" s="90"/>
+      <c r="V32" s="90"/>
       <c r="W32" s="5"/>
       <c r="X32" s="6"/>
       <c r="Z32" s="75">
@@ -4201,11 +4193,11 @@
       <c r="Z33" s="78">
         <v>1752</v>
       </c>
-      <c r="AA33" s="86" t="s">
+      <c r="AA33" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="AB33" s="86"/>
-      <c r="AC33" s="87"/>
+      <c r="AB33" s="91"/>
+      <c r="AC33" s="92"/>
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
@@ -4257,11 +4249,11 @@
         <f>Z32-Z33</f>
         <v>248</v>
       </c>
-      <c r="AA34" s="86" t="s">
+      <c r="AA34" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="AB34" s="86"/>
-      <c r="AC34" s="87"/>
+      <c r="AB34" s="91"/>
+      <c r="AC34" s="92"/>
     </row>
     <row r="35" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="18">
@@ -4573,13 +4565,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G1:M1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="T13:V13"/>
     <mergeCell ref="AA33:AC33"/>
     <mergeCell ref="AA34:AC34"/>
     <mergeCell ref="D23:F23"/>
@@ -4588,6 +4573,13 @@
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="L32:N32"/>
     <mergeCell ref="T32:V32"/>
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="T13:V13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X1" r:id="rId1" display="https://www.wincalendar.com/Calendar-and-Schedule-Templates" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Added formulas to cells to match with total hour of work per month
</commit_message>
<xml_diff>
--- a/2021.xlsx
+++ b/2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\Control-Horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B40504-AA7B-489E-AF30-F25CA0046B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD247BA-0316-4259-BF5F-F3FCB12760AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2682,8 +2682,8 @@
   </sheetPr>
   <dimension ref="B1:AC40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:M1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,10 +3145,6 @@
       <c r="M10" s="41"/>
       <c r="N10" s="41"/>
       <c r="O10" s="41"/>
-      <c r="P10" s="73">
-        <f>J10*8</f>
-        <v>160</v>
-      </c>
       <c r="R10" s="74">
         <v>23</v>
       </c>
@@ -3157,10 +3153,6 @@
       <c r="U10" s="41"/>
       <c r="V10" s="41"/>
       <c r="W10" s="41"/>
-      <c r="X10" s="74">
-        <f>R10*8</f>
-        <v>184</v>
-      </c>
       <c r="AA10" t="s">
         <v>29</v>
       </c>
@@ -3178,6 +3170,14 @@
         <f>B11*8</f>
         <v>152</v>
       </c>
+      <c r="P11" s="73">
+        <f>J10*8</f>
+        <v>160</v>
+      </c>
+      <c r="X11" s="74">
+        <f>R10*8</f>
+        <v>184</v>
+      </c>
       <c r="AA11" t="s">
         <v>31</v>
       </c>
@@ -3599,10 +3599,6 @@
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
-      <c r="H20" s="74">
-        <f>B20*8</f>
-        <v>160</v>
-      </c>
       <c r="J20" s="37">
         <v>44346</v>
       </c>
@@ -3622,12 +3618,12 @@
       <c r="U20" s="41"/>
       <c r="V20" s="41"/>
       <c r="W20" s="41"/>
-      <c r="X20" s="74">
-        <f>R20*8</f>
-        <v>160</v>
-      </c>
     </row>
     <row r="21" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H21" s="74">
+        <f>B20*8</f>
+        <v>160</v>
+      </c>
       <c r="J21" s="74">
         <v>21</v>
       </c>
@@ -3640,6 +3636,10 @@
         <f>J21*8</f>
         <v>168</v>
       </c>
+      <c r="X21" s="74">
+        <f>R20*8</f>
+        <v>160</v>
+      </c>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.3">
       <c r="Z22" s="70"/>
@@ -4117,7 +4117,7 @@
       <c r="W32" s="5"/>
       <c r="X32" s="6"/>
       <c r="Z32" s="75">
-        <f>H11+P10+X10+H20+P21+X20+H30+P30+X30+H40+P39+X39</f>
+        <f>H11+P11+X11+H21+P21+X21+H30+P30+X30+H40+P40+X40</f>
         <v>2000</v>
       </c>
       <c r="AA32" s="76" t="s">
@@ -4532,10 +4532,6 @@
       <c r="M39" s="41"/>
       <c r="N39" s="41"/>
       <c r="O39" s="41"/>
-      <c r="P39" s="74">
-        <f>J39*8</f>
-        <v>168</v>
-      </c>
       <c r="R39" s="74">
         <v>21</v>
       </c>
@@ -4544,10 +4540,6 @@
       <c r="U39" s="41"/>
       <c r="V39" s="41"/>
       <c r="W39" s="41"/>
-      <c r="X39" s="74">
-        <f>R39*8</f>
-        <v>168</v>
-      </c>
     </row>
     <row r="40" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="74">
@@ -4561,6 +4553,14 @@
       <c r="H40" s="74">
         <f>B40*8</f>
         <v>160</v>
+      </c>
+      <c r="P40" s="74">
+        <f>J39*8</f>
+        <v>168</v>
+      </c>
+      <c r="X40" s="74">
+        <f>R39*8</f>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>